<commit_message>
Added till 11/04/2021[Week 2 completed]
</commit_message>
<xml_diff>
--- a/Week 2/Week 2 Plan.xlsx
+++ b/Week 2/Week 2 Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSA\Week 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3175C69-BCE4-4832-B84B-5D0B63B343E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F11BBF3-AA46-4262-88A4-70866B324C78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
   <si>
     <t>Arrays and Matrices</t>
   </si>
@@ -610,8 +610,8 @@
   </sheetPr>
   <dimension ref="A1:Q1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1187,7 +1187,9 @@
       <c r="A26" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="12" t="s">
+        <v>58</v>
+      </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>

</xml_diff>